<commit_message>
fix nullable in plan visit
</commit_message>
<xml_diff>
--- a/public/import/outlet_template (12).xlsx
+++ b/public/import/outlet_template (12).xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\finance online\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WANDA FITRIANA PUTRI\SAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E26AE7-1E23-4AD0-9E3D-D1C0596DF8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B034E-5D0C-4843-9773-B95A015B7BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>badan_usaha</t>
   </si>
@@ -75,36 +75,63 @@
     <t>REALME</t>
   </si>
   <si>
+    <t>MAINTAIN</t>
+  </si>
+  <si>
+    <t>BIGCIREBON</t>
+  </si>
+  <si>
     <t>BIGKARAWANG</t>
   </si>
   <si>
-    <t>BT03764</t>
-  </si>
-  <si>
-    <t>STAR CELL</t>
-  </si>
-  <si>
-    <t>Jl Raya Sukanagara No 32, Cianjur</t>
-  </si>
-  <si>
-    <t>KAB CIANJUR</t>
-  </si>
-  <si>
-    <t>MAINTAIN</t>
-  </si>
-  <si>
-    <t>KRWASC1</t>
+    <t>CRBASC2</t>
+  </si>
+  <si>
+    <t>KRWASC3</t>
+  </si>
+  <si>
+    <t>BT03852</t>
+  </si>
+  <si>
+    <t>BIOHAZARD PHONE</t>
+  </si>
+  <si>
+    <t>jl pasar loji desa cinta laksana tegal waru karawang</t>
+  </si>
+  <si>
+    <t>KARAWANG 1</t>
+  </si>
+  <si>
+    <t>BT01153</t>
+  </si>
+  <si>
+    <t>GALAXY CELL</t>
+  </si>
+  <si>
+    <t>Ds Rambatan Wetan Blok Pecuk Katapang Rt 29/08 (Samping SMP Hidayatul Mujahidin) Indramayu</t>
+  </si>
+  <si>
+    <t>INDRAMAYU</t>
+  </si>
+  <si>
+    <t>UNMAINTAIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -127,8 +154,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,26 +514,55 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix export for data null in outlet
</commit_message>
<xml_diff>
--- a/public/import/outlet_template (12).xlsx
+++ b/public/import/outlet_template (12).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\WANDA FITRIANA PUTRI\SAM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3B034E-5D0C-4843-9773-B95A015B7BB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44293979-5B13-4C34-98AE-CCA480940971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>badan_usaha</t>
   </si>
@@ -69,52 +69,40 @@
     <t>latlong</t>
   </si>
   <si>
+    <t>MAINTAIN</t>
+  </si>
+  <si>
     <t>CV.TOP</t>
   </si>
   <si>
     <t>REALME</t>
   </si>
   <si>
-    <t>MAINTAIN</t>
-  </si>
-  <si>
-    <t>BIGCIREBON</t>
+    <t>BT07227</t>
+  </si>
+  <si>
+    <t>ALVIS CELL</t>
+  </si>
+  <si>
+    <t>JL MAYJEN SUTOYO NO 127 KEL. KARANGANYAR SUBANG</t>
+  </si>
+  <si>
+    <t>KOTA SUBANG</t>
   </si>
   <si>
     <t>BIGKARAWANG</t>
   </si>
   <si>
-    <t>CRBASC2</t>
-  </si>
-  <si>
-    <t>KRWASC3</t>
-  </si>
-  <si>
-    <t>BT03852</t>
-  </si>
-  <si>
-    <t>BIOHAZARD PHONE</t>
-  </si>
-  <si>
-    <t>jl pasar loji desa cinta laksana tegal waru karawang</t>
-  </si>
-  <si>
-    <t>KARAWANG 1</t>
-  </si>
-  <si>
-    <t>BT01153</t>
-  </si>
-  <si>
-    <t>GALAXY CELL</t>
-  </si>
-  <si>
-    <t>Ds Rambatan Wetan Blok Pecuk Katapang Rt 29/08 (Samping SMP Hidayatul Mujahidin) Indramayu</t>
-  </si>
-  <si>
-    <t>INDRAMAYU</t>
-  </si>
-  <si>
-    <t>UNMAINTAIN</t>
+    <t>KRWASC2</t>
+  </si>
+  <si>
+    <t>Jl. Otto Iskandardinata No.50 kel.karanganyar kec.subang kab.Subang</t>
+  </si>
+  <si>
+    <t>Raza Gadget Subang</t>
+  </si>
+  <si>
+    <t>008.345</t>
   </si>
 </sst>
 </file>
@@ -461,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,62 +496,155 @@
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
-      </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I28" s="1"/>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I29" s="1"/>
+    </row>
+    <row r="30" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I30" s="1"/>
+    </row>
+    <row r="31" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I31" s="1"/>
+    </row>
+    <row r="32" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I32" s="1"/>
+    </row>
+    <row r="33" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I33" s="1"/>
+    </row>
+    <row r="34" spans="9:9" x14ac:dyDescent="0.35">
+      <c r="I34" s="1"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>

</xml_diff>